<commit_message>
formatted the other spreadsheets for korvin
made everything consistent to avoid confusion
</commit_message>
<xml_diff>
--- a/Surveys/07_06_2022_Tracer_Survey.xlsx
+++ b/Surveys/07_06_2022_Tracer_Survey.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alfon\OneDrive\Escritorio\AUTOCADBIBI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicol\Documents\GitHub\RFID_tracers\Surveys\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7EC24DA-3A04-4550-8A9C-D01D4507B740}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E788BBAA-571D-46BC-A5CC-4ED2012E09F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A3AF3E8F-FEA9-4812-A076-230554F8424C}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="28">
   <si>
     <t>Tracer survey for trainagulating locations on streambed</t>
   </si>
@@ -85,40 +85,40 @@
     <t>Northing (Y)</t>
   </si>
   <si>
-    <t>no chocan</t>
+    <t>Coordinates</t>
   </si>
   <si>
-    <t>539902,540</t>
+    <t>Triangle Properties</t>
   </si>
   <si>
-    <t>539903,490</t>
+    <t>Error</t>
   </si>
   <si>
-    <t>475293,210</t>
+    <t>Area</t>
   </si>
   <si>
-    <t>475292,910</t>
+    <t>Perimeter</t>
   </si>
   <si>
-    <t>539954,750</t>
+    <t>H1</t>
   </si>
   <si>
-    <t>539955,100</t>
+    <t>H2</t>
   </si>
   <si>
-    <t>475232,410</t>
+    <t>H3</t>
   </si>
   <si>
-    <t>475233,600</t>
+    <t>A</t>
   </si>
   <si>
-    <t>475234,940</t>
+    <t>B</t>
   </si>
   <si>
-    <t>475238,990</t>
+    <t>C</t>
   </si>
   <si>
-    <t>475239,100</t>
+    <t>Composite Error</t>
   </si>
 </sst>
 </file>
@@ -148,7 +148,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="15">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -223,12 +223,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -274,7 +268,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -336,13 +330,10 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -363,28 +354,13 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="12" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="13" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="14" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -403,7 +379,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -699,13 +675,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A376C9C8-D535-4C27-86BF-35E3FAC570AB}">
-  <dimension ref="A1:I110"/>
+  <dimension ref="A1:O110"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I113" sqref="I109:I113"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G46" sqref="G46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="17.6640625" customWidth="1"/>
     <col min="2" max="2" width="16" customWidth="1"/>
@@ -714,29 +690,31 @@
     <col min="5" max="5" width="13.5546875" customWidth="1"/>
     <col min="6" max="6" width="15.44140625" customWidth="1"/>
     <col min="7" max="7" width="11.33203125" customWidth="1"/>
-    <col min="8" max="8" width="4.109375" customWidth="1"/>
+    <col min="8" max="8" width="15.21875" customWidth="1"/>
     <col min="9" max="9" width="14.109375" customWidth="1"/>
-    <col min="13" max="13" width="5" customWidth="1"/>
-    <col min="14" max="14" width="13.5546875" customWidth="1"/>
+    <col min="12" max="12" width="14.5546875" customWidth="1"/>
+    <col min="13" max="13" width="12.33203125" customWidth="1"/>
+    <col min="14" max="14" width="10.109375" customWidth="1"/>
+    <col min="15" max="15" width="20.6640625" customWidth="1"/>
     <col min="18" max="18" width="4.109375" customWidth="1"/>
     <col min="19" max="19" width="10.88671875" customWidth="1"/>
     <col min="23" max="23" width="4" customWidth="1"/>
     <col min="24" max="24" width="11.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="25" t="s">
+    <row r="1" spans="1:15" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="25"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B1" s="24"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>44748</v>
       </c>
       <c r="B2" s="2"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -744,7 +722,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -752,7 +730,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
@@ -760,18 +738,35 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="24.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="7" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" ht="24.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="7" spans="1:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="26" t="s">
+      <c r="B7" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="26"/>
-      <c r="D7" s="26"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C7" s="25"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" s="29"/>
+      <c r="G7" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="H7" s="29"/>
+      <c r="I7" s="29"/>
+      <c r="J7" s="29"/>
+      <c r="K7" s="29"/>
+      <c r="L7" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="M7" s="29"/>
+      <c r="N7" s="29"/>
+      <c r="O7" s="29"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
         <v>12</v>
       </c>
@@ -784,14 +779,41 @@
       <c r="D8" s="10">
         <v>12</v>
       </c>
-      <c r="E8" s="20" t="s">
+      <c r="E8" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="F8" s="20" t="s">
+      <c r="F8" s="30" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G8" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="H8" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="I8" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="J8" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="K8" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="L8" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="M8" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="N8" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="O8" s="21" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" s="11">
         <v>3</v>
       </c>
@@ -804,14 +826,19 @@
       <c r="D9" s="19">
         <v>121</v>
       </c>
-      <c r="E9" s="21">
-        <v>475295.22899999999</v>
-      </c>
-      <c r="F9" s="20">
-        <v>539904.86499999999</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E9" s="20"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="31"/>
+      <c r="H9" s="31"/>
+      <c r="I9" s="31"/>
+      <c r="J9" s="31"/>
+      <c r="K9" s="31"/>
+      <c r="L9" s="31"/>
+      <c r="M9" s="31"/>
+      <c r="N9" s="31"/>
+      <c r="O9" s="31"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" s="14">
         <v>113</v>
       </c>
@@ -820,8 +847,17 @@
       <c r="D10" s="12"/>
       <c r="E10" s="20"/>
       <c r="F10" s="20"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G10" s="31"/>
+      <c r="H10" s="31"/>
+      <c r="I10" s="31"/>
+      <c r="J10" s="31"/>
+      <c r="K10" s="31"/>
+      <c r="L10" s="31"/>
+      <c r="M10" s="31"/>
+      <c r="N10" s="31"/>
+      <c r="O10" s="31"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" s="13">
         <v>42</v>
       </c>
@@ -830,8 +866,17 @@
       <c r="D11" s="12"/>
       <c r="E11" s="20"/>
       <c r="F11" s="20"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G11" s="31"/>
+      <c r="H11" s="31"/>
+      <c r="I11" s="31"/>
+      <c r="J11" s="31"/>
+      <c r="K11" s="31"/>
+      <c r="L11" s="31"/>
+      <c r="M11" s="31"/>
+      <c r="N11" s="31"/>
+      <c r="O11" s="31"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" s="13">
         <v>4</v>
       </c>
@@ -844,14 +889,19 @@
       <c r="D12" s="12">
         <v>77</v>
       </c>
-      <c r="E12" s="20">
-        <v>475294.75699999998</v>
-      </c>
-      <c r="F12" s="20">
-        <v>539904.66200000001</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E12" s="20"/>
+      <c r="F12" s="20"/>
+      <c r="G12" s="31"/>
+      <c r="H12" s="31"/>
+      <c r="I12" s="31"/>
+      <c r="J12" s="31"/>
+      <c r="K12" s="31"/>
+      <c r="L12" s="31"/>
+      <c r="M12" s="31"/>
+      <c r="N12" s="31"/>
+      <c r="O12" s="31"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" s="15">
         <v>105</v>
       </c>
@@ -864,14 +914,19 @@
       <c r="D13" s="12">
         <v>77</v>
       </c>
-      <c r="E13" s="30">
-        <v>475294.53600000002</v>
-      </c>
-      <c r="F13" s="30">
-        <v>539904.79099999997</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E13" s="20"/>
+      <c r="F13" s="20"/>
+      <c r="G13" s="31"/>
+      <c r="H13" s="31"/>
+      <c r="I13" s="31"/>
+      <c r="J13" s="31"/>
+      <c r="K13" s="31"/>
+      <c r="L13" s="31"/>
+      <c r="M13" s="31"/>
+      <c r="N13" s="31"/>
+      <c r="O13" s="31"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" s="15">
         <v>25</v>
       </c>
@@ -884,14 +939,19 @@
       <c r="D14" s="12">
         <v>129</v>
       </c>
-      <c r="E14" s="30">
-        <v>475294.76899999997</v>
-      </c>
-      <c r="F14" s="30">
-        <v>539905.21499999997</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E14" s="20"/>
+      <c r="F14" s="20"/>
+      <c r="G14" s="31"/>
+      <c r="H14" s="31"/>
+      <c r="I14" s="31"/>
+      <c r="J14" s="31"/>
+      <c r="K14" s="31"/>
+      <c r="L14" s="31"/>
+      <c r="M14" s="31"/>
+      <c r="N14" s="31"/>
+      <c r="O14" s="31"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" s="15">
         <v>30</v>
       </c>
@@ -904,14 +964,19 @@
       <c r="D15" s="12">
         <v>113</v>
       </c>
-      <c r="E15" s="30">
-        <v>475294.06800000003</v>
-      </c>
-      <c r="F15" s="30">
-        <v>539905.09400000004</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E15" s="20"/>
+      <c r="F15" s="20"/>
+      <c r="G15" s="31"/>
+      <c r="H15" s="31"/>
+      <c r="I15" s="31"/>
+      <c r="J15" s="31"/>
+      <c r="K15" s="31"/>
+      <c r="L15" s="31"/>
+      <c r="M15" s="31"/>
+      <c r="N15" s="31"/>
+      <c r="O15" s="31"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16" s="15">
         <v>99</v>
       </c>
@@ -924,13 +989,19 @@
       <c r="D16" s="12">
         <v>74</v>
       </c>
-      <c r="E16" s="31"/>
-      <c r="F16" s="30"/>
-      <c r="G16" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E16" s="20"/>
+      <c r="F16" s="20"/>
+      <c r="G16" s="31"/>
+      <c r="H16" s="31"/>
+      <c r="I16" s="31"/>
+      <c r="J16" s="31"/>
+      <c r="K16" s="31"/>
+      <c r="L16" s="31"/>
+      <c r="M16" s="31"/>
+      <c r="N16" s="31"/>
+      <c r="O16" s="31"/>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A17" s="16">
         <v>33</v>
       </c>
@@ -943,14 +1014,19 @@
       <c r="D17" s="12">
         <v>137</v>
       </c>
-      <c r="E17" s="30">
-        <v>475293.45400000003</v>
-      </c>
-      <c r="F17" s="30">
-        <v>539902.98800000001</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E17" s="22"/>
+      <c r="F17" s="20"/>
+      <c r="G17" s="31"/>
+      <c r="H17" s="31"/>
+      <c r="I17" s="31"/>
+      <c r="J17" s="31"/>
+      <c r="K17" s="31"/>
+      <c r="L17" s="31"/>
+      <c r="M17" s="31"/>
+      <c r="N17" s="31"/>
+      <c r="O17" s="31"/>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A18" s="16">
         <v>117</v>
       </c>
@@ -963,14 +1039,19 @@
       <c r="D18" s="12">
         <v>153</v>
       </c>
-      <c r="E18" s="30">
-        <v>475295.413</v>
-      </c>
-      <c r="F18" s="30">
-        <v>539905.098</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E18" s="20"/>
+      <c r="F18" s="20"/>
+      <c r="G18" s="31"/>
+      <c r="H18" s="31"/>
+      <c r="I18" s="31"/>
+      <c r="J18" s="31"/>
+      <c r="K18" s="31"/>
+      <c r="L18" s="31"/>
+      <c r="M18" s="31"/>
+      <c r="N18" s="31"/>
+      <c r="O18" s="31"/>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A19" s="16">
         <v>26</v>
       </c>
@@ -983,24 +1064,38 @@
       <c r="D19" s="12">
         <v>158</v>
       </c>
-      <c r="E19" s="30">
-        <v>475293.84899999999</v>
-      </c>
-      <c r="F19" s="30">
-        <v>539902.65700000001</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E19" s="20"/>
+      <c r="F19" s="20"/>
+      <c r="G19" s="31"/>
+      <c r="H19" s="31"/>
+      <c r="I19" s="31"/>
+      <c r="J19" s="31"/>
+      <c r="K19" s="31"/>
+      <c r="L19" s="31"/>
+      <c r="M19" s="31"/>
+      <c r="N19" s="31"/>
+      <c r="O19" s="31"/>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A20" s="16">
         <v>54</v>
       </c>
       <c r="B20" s="12"/>
       <c r="C20" s="12"/>
       <c r="D20" s="12"/>
-      <c r="E20" s="30"/>
-      <c r="F20" s="30"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E20" s="20"/>
+      <c r="F20" s="20"/>
+      <c r="G20" s="31"/>
+      <c r="H20" s="31"/>
+      <c r="I20" s="31"/>
+      <c r="J20" s="31"/>
+      <c r="K20" s="31"/>
+      <c r="L20" s="31"/>
+      <c r="M20" s="31"/>
+      <c r="N20" s="31"/>
+      <c r="O20" s="31"/>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A21" s="16">
         <v>55</v>
       </c>
@@ -1013,44 +1108,76 @@
       <c r="D21" s="12">
         <v>143</v>
       </c>
-      <c r="E21" s="30">
-        <v>475293.06400000001</v>
-      </c>
-      <c r="F21" s="30">
-        <v>539904.33100000001</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E21" s="20"/>
+      <c r="F21" s="20"/>
+      <c r="G21" s="31"/>
+      <c r="H21" s="31"/>
+      <c r="I21" s="31"/>
+      <c r="J21" s="31"/>
+      <c r="K21" s="31"/>
+      <c r="L21" s="31"/>
+      <c r="M21" s="31"/>
+      <c r="N21" s="31"/>
+      <c r="O21" s="31"/>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A22" s="17">
         <v>71</v>
       </c>
       <c r="B22" s="12"/>
       <c r="C22" s="12"/>
       <c r="D22" s="12"/>
-      <c r="E22" s="30"/>
-      <c r="F22" s="30"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E22" s="20"/>
+      <c r="F22" s="20"/>
+      <c r="G22" s="31"/>
+      <c r="H22" s="31"/>
+      <c r="I22" s="31"/>
+      <c r="J22" s="31"/>
+      <c r="K22" s="31"/>
+      <c r="L22" s="31"/>
+      <c r="M22" s="31"/>
+      <c r="N22" s="31"/>
+      <c r="O22" s="31"/>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A23" s="17">
         <v>51</v>
       </c>
       <c r="B23" s="12"/>
       <c r="C23" s="12"/>
       <c r="D23" s="12"/>
-      <c r="E23" s="30"/>
-      <c r="F23" s="30"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E23" s="20"/>
+      <c r="F23" s="20"/>
+      <c r="G23" s="31"/>
+      <c r="H23" s="31"/>
+      <c r="I23" s="31"/>
+      <c r="J23" s="31"/>
+      <c r="K23" s="31"/>
+      <c r="L23" s="31"/>
+      <c r="M23" s="31"/>
+      <c r="N23" s="31"/>
+      <c r="O23" s="31"/>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A24" s="17">
         <v>80</v>
       </c>
       <c r="B24" s="12"/>
       <c r="C24" s="12"/>
       <c r="D24" s="12"/>
-      <c r="E24" s="30"/>
-      <c r="F24" s="30"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E24" s="20"/>
+      <c r="F24" s="20"/>
+      <c r="G24" s="31"/>
+      <c r="H24" s="31"/>
+      <c r="I24" s="31"/>
+      <c r="J24" s="31"/>
+      <c r="K24" s="31"/>
+      <c r="L24" s="31"/>
+      <c r="M24" s="31"/>
+      <c r="N24" s="31"/>
+      <c r="O24" s="31"/>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A25" s="17">
         <v>63</v>
       </c>
@@ -1063,15 +1190,19 @@
       <c r="D25" s="12">
         <v>130</v>
       </c>
-      <c r="E25" s="30">
-        <v>475293.33299999998</v>
-      </c>
-      <c r="F25" s="30">
-        <v>539903.19799999997</v>
-      </c>
-      <c r="G25" s="2"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E25" s="20"/>
+      <c r="F25" s="20"/>
+      <c r="G25" s="31"/>
+      <c r="H25" s="31"/>
+      <c r="I25" s="31"/>
+      <c r="J25" s="31"/>
+      <c r="K25" s="31"/>
+      <c r="L25" s="31"/>
+      <c r="M25" s="31"/>
+      <c r="N25" s="31"/>
+      <c r="O25" s="31"/>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A26" s="17">
         <v>87</v>
       </c>
@@ -1084,13 +1215,19 @@
       <c r="D26" s="12">
         <v>66</v>
       </c>
-      <c r="E26" s="30"/>
-      <c r="F26" s="30"/>
-      <c r="G26" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E26" s="20"/>
+      <c r="F26" s="20"/>
+      <c r="G26" s="31"/>
+      <c r="H26" s="31"/>
+      <c r="I26" s="31"/>
+      <c r="J26" s="31"/>
+      <c r="K26" s="31"/>
+      <c r="L26" s="31"/>
+      <c r="M26" s="31"/>
+      <c r="N26" s="31"/>
+      <c r="O26" s="31"/>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A27" s="17">
         <v>50</v>
       </c>
@@ -1099,8 +1236,17 @@
       <c r="D27" s="12"/>
       <c r="E27" s="20"/>
       <c r="F27" s="20"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G27" s="31"/>
+      <c r="H27" s="31"/>
+      <c r="I27" s="31"/>
+      <c r="J27" s="31"/>
+      <c r="K27" s="31"/>
+      <c r="L27" s="31"/>
+      <c r="M27" s="31"/>
+      <c r="N27" s="31"/>
+      <c r="O27" s="31"/>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A28" s="17">
         <v>26</v>
       </c>
@@ -1113,14 +1259,19 @@
       <c r="D28" s="12">
         <v>153</v>
       </c>
-      <c r="E28" s="30">
-        <v>475293.73100000003</v>
-      </c>
-      <c r="F28" s="30">
-        <v>539902.61800000002</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E28" s="20"/>
+      <c r="F28" s="20"/>
+      <c r="G28" s="31"/>
+      <c r="H28" s="31"/>
+      <c r="I28" s="31"/>
+      <c r="J28" s="31"/>
+      <c r="K28" s="31"/>
+      <c r="L28" s="31"/>
+      <c r="M28" s="31"/>
+      <c r="N28" s="31"/>
+      <c r="O28" s="31"/>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A29" s="17">
         <v>55</v>
       </c>
@@ -1133,14 +1284,19 @@
       <c r="D29" s="12">
         <v>173</v>
       </c>
-      <c r="E29" s="30">
-        <v>475293.505</v>
-      </c>
-      <c r="F29" s="30">
-        <v>539902.49300000002</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E29" s="20"/>
+      <c r="F29" s="20"/>
+      <c r="G29" s="31"/>
+      <c r="H29" s="31"/>
+      <c r="I29" s="31"/>
+      <c r="J29" s="31"/>
+      <c r="K29" s="31"/>
+      <c r="L29" s="31"/>
+      <c r="M29" s="31"/>
+      <c r="N29" s="31"/>
+      <c r="O29" s="31"/>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A30" s="17">
         <v>37</v>
       </c>
@@ -1149,18 +1305,44 @@
       <c r="D30" s="12"/>
       <c r="E30" s="20"/>
       <c r="F30" s="20"/>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G30" s="31"/>
+      <c r="H30" s="31"/>
+      <c r="I30" s="31"/>
+      <c r="J30" s="31"/>
+      <c r="K30" s="31"/>
+      <c r="L30" s="31"/>
+      <c r="M30" s="31"/>
+      <c r="N30" s="31"/>
+      <c r="O30" s="31"/>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A32" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B32" s="27" t="s">
+      <c r="B32" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="C32" s="27"/>
-      <c r="D32" s="27"/>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C32" s="26"/>
+      <c r="D32" s="26"/>
+      <c r="E32" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="F32" s="29"/>
+      <c r="G32" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="H32" s="29"/>
+      <c r="I32" s="29"/>
+      <c r="J32" s="29"/>
+      <c r="K32" s="29"/>
+      <c r="L32" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="M32" s="29"/>
+      <c r="N32" s="29"/>
+      <c r="O32" s="29"/>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A33" s="10" t="s">
         <v>12</v>
       </c>
@@ -1173,14 +1355,41 @@
       <c r="D33" s="10">
         <v>12</v>
       </c>
-      <c r="E33" s="20" t="s">
+      <c r="E33" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="F33" s="20" t="s">
+      <c r="F33" s="30" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G33" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="H33" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="I33" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="J33" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="K33" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="L33" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="M33" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="N33" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="O33" s="21" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A34" s="11">
         <v>7</v>
       </c>
@@ -1193,14 +1402,19 @@
       <c r="D34" s="12">
         <v>194</v>
       </c>
-      <c r="E34" s="30">
-        <v>475292.73800000001</v>
-      </c>
-      <c r="F34" s="30">
-        <v>539902.96900000004</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E34" s="20"/>
+      <c r="F34" s="20"/>
+      <c r="G34" s="31"/>
+      <c r="H34" s="31"/>
+      <c r="I34" s="31"/>
+      <c r="J34" s="31"/>
+      <c r="K34" s="31"/>
+      <c r="L34" s="31"/>
+      <c r="M34" s="31"/>
+      <c r="N34" s="31"/>
+      <c r="O34" s="31"/>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A35" s="13">
         <v>44</v>
       </c>
@@ -1213,14 +1427,19 @@
       <c r="D35" s="12">
         <v>168</v>
       </c>
-      <c r="E35" s="30">
-        <v>475293.022</v>
-      </c>
-      <c r="F35" s="30">
-        <v>539902.98499999999</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E35" s="20"/>
+      <c r="F35" s="20"/>
+      <c r="G35" s="31"/>
+      <c r="H35" s="31"/>
+      <c r="I35" s="31"/>
+      <c r="J35" s="31"/>
+      <c r="K35" s="31"/>
+      <c r="L35" s="31"/>
+      <c r="M35" s="31"/>
+      <c r="N35" s="31"/>
+      <c r="O35" s="31"/>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A36" s="15">
         <v>13</v>
       </c>
@@ -1233,14 +1452,19 @@
       <c r="D36" s="12">
         <v>155</v>
       </c>
-      <c r="E36" s="30">
-        <v>475292.93300000002</v>
-      </c>
-      <c r="F36" s="30">
-        <v>539903.44200000004</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E36" s="20"/>
+      <c r="F36" s="20"/>
+      <c r="G36" s="31"/>
+      <c r="H36" s="31"/>
+      <c r="I36" s="31"/>
+      <c r="J36" s="31"/>
+      <c r="K36" s="31"/>
+      <c r="L36" s="31"/>
+      <c r="M36" s="31"/>
+      <c r="N36" s="31"/>
+      <c r="O36" s="31"/>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A37" s="15">
         <v>16</v>
       </c>
@@ -1253,14 +1477,19 @@
       <c r="D37" s="12">
         <v>180</v>
       </c>
-      <c r="E37" s="30">
-        <v>475292.81699999998</v>
-      </c>
-      <c r="F37" s="30">
-        <v>539903.08700000006</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E37" s="20"/>
+      <c r="F37" s="20"/>
+      <c r="G37" s="31"/>
+      <c r="H37" s="31"/>
+      <c r="I37" s="31"/>
+      <c r="J37" s="31"/>
+      <c r="K37" s="31"/>
+      <c r="L37" s="31"/>
+      <c r="M37" s="31"/>
+      <c r="N37" s="31"/>
+      <c r="O37" s="31"/>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A38" s="15">
         <v>112</v>
       </c>
@@ -1273,14 +1502,19 @@
       <c r="D38" s="12">
         <v>227</v>
       </c>
-      <c r="E38" s="30">
-        <v>475292.62599999999</v>
-      </c>
-      <c r="F38" s="32" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E38" s="20"/>
+      <c r="F38" s="20"/>
+      <c r="G38" s="31"/>
+      <c r="H38" s="31"/>
+      <c r="I38" s="31"/>
+      <c r="J38" s="31"/>
+      <c r="K38" s="31"/>
+      <c r="L38" s="31"/>
+      <c r="M38" s="31"/>
+      <c r="N38" s="31"/>
+      <c r="O38" s="31"/>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A39" s="16">
         <v>32</v>
       </c>
@@ -1293,14 +1527,19 @@
       <c r="D39" s="12">
         <v>233</v>
       </c>
-      <c r="E39" s="30">
-        <v>475292.73100000003</v>
-      </c>
-      <c r="F39" s="30">
-        <v>539902.32799999998</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E39" s="20"/>
+      <c r="F39" s="20"/>
+      <c r="G39" s="31"/>
+      <c r="H39" s="31"/>
+      <c r="I39" s="31"/>
+      <c r="J39" s="31"/>
+      <c r="K39" s="31"/>
+      <c r="L39" s="31"/>
+      <c r="M39" s="31"/>
+      <c r="N39" s="31"/>
+      <c r="O39" s="31"/>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A40" s="16">
         <v>59</v>
       </c>
@@ -1313,14 +1552,19 @@
       <c r="D40" s="12">
         <v>169</v>
       </c>
-      <c r="E40" s="30">
-        <v>475292.76299999998</v>
-      </c>
-      <c r="F40" s="32" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E40" s="20"/>
+      <c r="F40" s="20"/>
+      <c r="G40" s="31"/>
+      <c r="H40" s="31"/>
+      <c r="I40" s="31"/>
+      <c r="J40" s="31"/>
+      <c r="K40" s="31"/>
+      <c r="L40" s="31"/>
+      <c r="M40" s="31"/>
+      <c r="N40" s="31"/>
+      <c r="O40" s="31"/>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A41" s="16">
         <v>57</v>
       </c>
@@ -1333,14 +1577,19 @@
       <c r="D41" s="12">
         <v>217</v>
       </c>
-      <c r="E41" s="31">
-        <v>475292.93599999999</v>
-      </c>
-      <c r="F41" s="30">
-        <v>539902.353</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E41" s="20"/>
+      <c r="F41" s="20"/>
+      <c r="G41" s="31"/>
+      <c r="H41" s="31"/>
+      <c r="I41" s="31"/>
+      <c r="J41" s="31"/>
+      <c r="K41" s="31"/>
+      <c r="L41" s="31"/>
+      <c r="M41" s="31"/>
+      <c r="N41" s="31"/>
+      <c r="O41" s="31"/>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A42" s="16">
         <v>104</v>
       </c>
@@ -1353,14 +1602,19 @@
       <c r="D42" s="12">
         <v>134</v>
       </c>
-      <c r="E42" s="32" t="s">
-        <v>19</v>
-      </c>
-      <c r="F42" s="30">
-        <v>539903.321</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E42" s="22"/>
+      <c r="F42" s="20"/>
+      <c r="G42" s="31"/>
+      <c r="H42" s="31"/>
+      <c r="I42" s="31"/>
+      <c r="J42" s="31"/>
+      <c r="K42" s="31"/>
+      <c r="L42" s="31"/>
+      <c r="M42" s="31"/>
+      <c r="N42" s="31"/>
+      <c r="O42" s="31"/>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A43" s="17">
         <v>127</v>
       </c>
@@ -1373,14 +1627,19 @@
       <c r="D43" s="12">
         <v>172</v>
       </c>
-      <c r="E43" s="30">
-        <v>475292.897</v>
-      </c>
-      <c r="F43" s="30">
-        <v>539903.11800000002</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E43" s="20"/>
+      <c r="F43" s="20"/>
+      <c r="G43" s="31"/>
+      <c r="H43" s="31"/>
+      <c r="I43" s="31"/>
+      <c r="J43" s="31"/>
+      <c r="K43" s="31"/>
+      <c r="L43" s="31"/>
+      <c r="M43" s="31"/>
+      <c r="N43" s="31"/>
+      <c r="O43" s="31"/>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A44" s="17">
         <v>134</v>
       </c>
@@ -1393,14 +1652,19 @@
       <c r="D44" s="12">
         <v>186</v>
       </c>
-      <c r="E44" s="30">
-        <v>475292.97100000002</v>
-      </c>
-      <c r="F44" s="30">
-        <v>539902.75600000005</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E44" s="20"/>
+      <c r="F44" s="20"/>
+      <c r="G44" s="31"/>
+      <c r="H44" s="31"/>
+      <c r="I44" s="31"/>
+      <c r="J44" s="31"/>
+      <c r="K44" s="31"/>
+      <c r="L44" s="31"/>
+      <c r="M44" s="31"/>
+      <c r="N44" s="31"/>
+      <c r="O44" s="31"/>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A45" s="17">
         <v>79</v>
       </c>
@@ -1413,15 +1677,19 @@
       <c r="D45" s="12">
         <v>220</v>
       </c>
-      <c r="E45" s="30">
-        <v>475292.65899999999</v>
-      </c>
-      <c r="F45" s="30">
-        <v>539902.60199999996</v>
-      </c>
-      <c r="I45" s="33"/>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E45" s="20"/>
+      <c r="F45" s="20"/>
+      <c r="G45" s="31"/>
+      <c r="H45" s="31"/>
+      <c r="I45" s="31"/>
+      <c r="J45" s="31"/>
+      <c r="K45" s="31"/>
+      <c r="L45" s="31"/>
+      <c r="M45" s="31"/>
+      <c r="N45" s="31"/>
+      <c r="O45" s="31"/>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A46" s="18">
         <v>17</v>
       </c>
@@ -1434,14 +1702,19 @@
       <c r="D46" s="12">
         <v>205</v>
       </c>
-      <c r="E46" s="30">
-        <v>475292.74800000002</v>
-      </c>
-      <c r="F46" s="30">
-        <v>539902.75699999998</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E46" s="20"/>
+      <c r="F46" s="20"/>
+      <c r="G46" s="31"/>
+      <c r="H46" s="31"/>
+      <c r="I46" s="31"/>
+      <c r="J46" s="31"/>
+      <c r="K46" s="31"/>
+      <c r="L46" s="31"/>
+      <c r="M46" s="31"/>
+      <c r="N46" s="31"/>
+      <c r="O46" s="31"/>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A47" s="18">
         <v>36</v>
       </c>
@@ -1454,14 +1727,19 @@
       <c r="D47" s="12">
         <v>220</v>
       </c>
-      <c r="E47" s="32" t="s">
-        <v>20</v>
-      </c>
-      <c r="F47" s="30">
-        <v>539902.35499999998</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E47" s="20"/>
+      <c r="F47" s="20"/>
+      <c r="G47" s="31"/>
+      <c r="H47" s="31"/>
+      <c r="I47" s="31"/>
+      <c r="J47" s="31"/>
+      <c r="K47" s="31"/>
+      <c r="L47" s="31"/>
+      <c r="M47" s="31"/>
+      <c r="N47" s="31"/>
+      <c r="O47" s="31"/>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A48" s="18">
         <v>44</v>
       </c>
@@ -1474,14 +1752,19 @@
       <c r="D48" s="12">
         <v>185</v>
       </c>
-      <c r="E48" s="30">
-        <v>475292.90399999998</v>
-      </c>
-      <c r="F48" s="30">
-        <v>539902.85800000001</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E48" s="20"/>
+      <c r="F48" s="20"/>
+      <c r="G48" s="31"/>
+      <c r="H48" s="31"/>
+      <c r="I48" s="31"/>
+      <c r="J48" s="31"/>
+      <c r="K48" s="31"/>
+      <c r="L48" s="31"/>
+      <c r="M48" s="31"/>
+      <c r="N48" s="31"/>
+      <c r="O48" s="31"/>
+    </row>
+    <row r="49" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A49" s="18">
         <v>65</v>
       </c>
@@ -1494,24 +1777,46 @@
       <c r="D49" s="12">
         <v>199</v>
       </c>
-      <c r="E49" s="30">
-        <v>475292.82299999997</v>
-      </c>
-      <c r="F49" s="30">
-        <v>539902.745</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E49" s="20"/>
+      <c r="F49" s="20"/>
+      <c r="G49" s="31"/>
+      <c r="H49" s="31"/>
+      <c r="I49" s="31"/>
+      <c r="J49" s="31"/>
+      <c r="K49" s="31"/>
+      <c r="L49" s="31"/>
+      <c r="M49" s="31"/>
+      <c r="N49" s="31"/>
+      <c r="O49" s="31"/>
+    </row>
+    <row r="51" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A51" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B51" s="28" t="s">
+      <c r="B51" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="C51" s="28"/>
-      <c r="D51" s="28"/>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C51" s="27"/>
+      <c r="D51" s="27"/>
+      <c r="E51" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="F51" s="29"/>
+      <c r="G51" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="H51" s="29"/>
+      <c r="I51" s="29"/>
+      <c r="J51" s="29"/>
+      <c r="K51" s="29"/>
+      <c r="L51" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="M51" s="29"/>
+      <c r="N51" s="29"/>
+      <c r="O51" s="29"/>
+    </row>
+    <row r="52" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A52" s="10" t="s">
         <v>12</v>
       </c>
@@ -1524,14 +1829,41 @@
       <c r="D52" s="10">
         <v>15</v>
       </c>
-      <c r="E52" s="22" t="s">
+      <c r="E52" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="F52" s="22" t="s">
+      <c r="F52" s="30" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G52" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="H52" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="I52" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="J52" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="K52" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="L52" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="M52" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="N52" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="O52" s="21" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="53" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A53" s="13">
         <v>22</v>
       </c>
@@ -1544,14 +1876,19 @@
       <c r="D53" s="19">
         <v>437</v>
       </c>
-      <c r="E53" s="34">
-        <v>475233.76699999999</v>
-      </c>
-      <c r="F53" s="34">
-        <v>539955.72699999996</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E53" s="20"/>
+      <c r="F53" s="20"/>
+      <c r="G53" s="31"/>
+      <c r="H53" s="31"/>
+      <c r="I53" s="31"/>
+      <c r="J53" s="31"/>
+      <c r="K53" s="31"/>
+      <c r="L53" s="31"/>
+      <c r="M53" s="31"/>
+      <c r="N53" s="31"/>
+      <c r="O53" s="31"/>
+    </row>
+    <row r="54" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A54" s="13">
         <v>114</v>
       </c>
@@ -1564,14 +1901,19 @@
       <c r="D54" s="12">
         <v>306</v>
       </c>
-      <c r="E54" s="34">
-        <v>475232.23499999999</v>
-      </c>
-      <c r="F54" s="34">
-        <v>539954.96499999997</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E54" s="20"/>
+      <c r="F54" s="20"/>
+      <c r="G54" s="31"/>
+      <c r="H54" s="31"/>
+      <c r="I54" s="31"/>
+      <c r="J54" s="31"/>
+      <c r="K54" s="31"/>
+      <c r="L54" s="31"/>
+      <c r="M54" s="31"/>
+      <c r="N54" s="31"/>
+      <c r="O54" s="31"/>
+    </row>
+    <row r="55" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A55" s="15">
         <v>90</v>
       </c>
@@ -1584,14 +1926,19 @@
       <c r="D55" s="12">
         <v>301</v>
       </c>
-      <c r="E55" s="34">
-        <v>475232.76799999998</v>
-      </c>
-      <c r="F55" s="35" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E55" s="20"/>
+      <c r="F55" s="20"/>
+      <c r="G55" s="31"/>
+      <c r="H55" s="31"/>
+      <c r="I55" s="31"/>
+      <c r="J55" s="31"/>
+      <c r="K55" s="31"/>
+      <c r="L55" s="31"/>
+      <c r="M55" s="31"/>
+      <c r="N55" s="31"/>
+      <c r="O55" s="31"/>
+    </row>
+    <row r="56" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A56" s="15">
         <v>19</v>
       </c>
@@ -1604,14 +1951,19 @@
       <c r="D56" s="12">
         <v>362</v>
       </c>
-      <c r="E56" s="34">
-        <v>475233.30300000001</v>
-      </c>
-      <c r="F56" s="34">
-        <v>539955.16500000004</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E56" s="20"/>
+      <c r="F56" s="20"/>
+      <c r="G56" s="31"/>
+      <c r="H56" s="31"/>
+      <c r="I56" s="31"/>
+      <c r="J56" s="31"/>
+      <c r="K56" s="31"/>
+      <c r="L56" s="31"/>
+      <c r="M56" s="31"/>
+      <c r="N56" s="31"/>
+      <c r="O56" s="31"/>
+    </row>
+    <row r="57" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A57" s="15">
         <v>106</v>
       </c>
@@ -1624,14 +1976,19 @@
       <c r="D57" s="12">
         <v>340</v>
       </c>
-      <c r="E57" s="34">
-        <v>475232.94199999998</v>
-      </c>
-      <c r="F57" s="35" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E57" s="20"/>
+      <c r="F57" s="20"/>
+      <c r="G57" s="31"/>
+      <c r="H57" s="31"/>
+      <c r="I57" s="31"/>
+      <c r="J57" s="31"/>
+      <c r="K57" s="31"/>
+      <c r="L57" s="31"/>
+      <c r="M57" s="31"/>
+      <c r="N57" s="31"/>
+      <c r="O57" s="31"/>
+    </row>
+    <row r="58" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A58" s="16">
         <v>49</v>
       </c>
@@ -1644,14 +2001,19 @@
       <c r="D58" s="12">
         <v>317</v>
       </c>
-      <c r="E58" s="34">
-        <v>475232.82699999999</v>
-      </c>
-      <c r="F58" s="34">
-        <v>539954.89800000004</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E58" s="20"/>
+      <c r="F58" s="20"/>
+      <c r="G58" s="31"/>
+      <c r="H58" s="31"/>
+      <c r="I58" s="31"/>
+      <c r="J58" s="31"/>
+      <c r="K58" s="31"/>
+      <c r="L58" s="31"/>
+      <c r="M58" s="31"/>
+      <c r="N58" s="31"/>
+      <c r="O58" s="31"/>
+    </row>
+    <row r="59" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A59" s="16">
         <v>128</v>
       </c>
@@ -1664,13 +2026,19 @@
       <c r="D59" s="12">
         <v>284</v>
       </c>
-      <c r="E59" s="22"/>
-      <c r="F59" s="22"/>
-      <c r="G59" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E59" s="20"/>
+      <c r="F59" s="20"/>
+      <c r="G59" s="31"/>
+      <c r="H59" s="31"/>
+      <c r="I59" s="31"/>
+      <c r="J59" s="31"/>
+      <c r="K59" s="31"/>
+      <c r="L59" s="31"/>
+      <c r="M59" s="31"/>
+      <c r="N59" s="31"/>
+      <c r="O59" s="31"/>
+    </row>
+    <row r="60" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A60" s="16">
         <v>47</v>
       </c>
@@ -1683,14 +2051,19 @@
       <c r="D60" s="12">
         <v>329</v>
       </c>
-      <c r="E60" s="34">
-        <v>475233.25300000003</v>
-      </c>
-      <c r="F60" s="34">
-        <v>539954.75699999998</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E60" s="20"/>
+      <c r="F60" s="20"/>
+      <c r="G60" s="31"/>
+      <c r="H60" s="31"/>
+      <c r="I60" s="31"/>
+      <c r="J60" s="31"/>
+      <c r="K60" s="31"/>
+      <c r="L60" s="31"/>
+      <c r="M60" s="31"/>
+      <c r="N60" s="31"/>
+      <c r="O60" s="31"/>
+    </row>
+    <row r="61" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A61" s="16">
         <v>39</v>
       </c>
@@ -1703,14 +2076,19 @@
       <c r="D61" s="12">
         <v>398</v>
       </c>
-      <c r="E61" s="34">
-        <v>475233.08399999997</v>
-      </c>
-      <c r="F61" s="34">
-        <v>539955.42500000005</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E61" s="22"/>
+      <c r="F61" s="20"/>
+      <c r="G61" s="31"/>
+      <c r="H61" s="31"/>
+      <c r="I61" s="31"/>
+      <c r="J61" s="31"/>
+      <c r="K61" s="31"/>
+      <c r="L61" s="31"/>
+      <c r="M61" s="31"/>
+      <c r="N61" s="31"/>
+      <c r="O61" s="31"/>
+    </row>
+    <row r="62" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A62" s="16">
         <v>120</v>
       </c>
@@ -1723,14 +2101,19 @@
       <c r="D62" s="12">
         <v>248</v>
       </c>
-      <c r="E62" s="35" t="s">
-        <v>23</v>
-      </c>
-      <c r="F62" s="34">
-        <v>539954.23300000001</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E62" s="20"/>
+      <c r="F62" s="20"/>
+      <c r="G62" s="31"/>
+      <c r="H62" s="31"/>
+      <c r="I62" s="31"/>
+      <c r="J62" s="31"/>
+      <c r="K62" s="31"/>
+      <c r="L62" s="31"/>
+      <c r="M62" s="31"/>
+      <c r="N62" s="31"/>
+      <c r="O62" s="31"/>
+    </row>
+    <row r="63" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A63" s="16" t="s">
         <v>13</v>
       </c>
@@ -1743,14 +2126,19 @@
       <c r="D63" s="12">
         <v>248</v>
       </c>
-      <c r="E63" s="35" t="s">
-        <v>23</v>
-      </c>
-      <c r="F63" s="34">
-        <v>539954.23300000001</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E63" s="20"/>
+      <c r="F63" s="20"/>
+      <c r="G63" s="31"/>
+      <c r="H63" s="31"/>
+      <c r="I63" s="31"/>
+      <c r="J63" s="31"/>
+      <c r="K63" s="31"/>
+      <c r="L63" s="31"/>
+      <c r="M63" s="31"/>
+      <c r="N63" s="31"/>
+      <c r="O63" s="31"/>
+    </row>
+    <row r="64" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A64" s="17">
         <v>130</v>
       </c>
@@ -1763,14 +2151,19 @@
       <c r="D64" s="12">
         <v>339</v>
       </c>
-      <c r="E64" s="34">
-        <v>475233.03499999997</v>
-      </c>
-      <c r="F64" s="34">
-        <v>539954.98800000001</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E64" s="20"/>
+      <c r="F64" s="20"/>
+      <c r="G64" s="31"/>
+      <c r="H64" s="31"/>
+      <c r="I64" s="31"/>
+      <c r="J64" s="31"/>
+      <c r="K64" s="31"/>
+      <c r="L64" s="31"/>
+      <c r="M64" s="31"/>
+      <c r="N64" s="31"/>
+      <c r="O64" s="31"/>
+    </row>
+    <row r="65" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A65" s="17">
         <v>123</v>
       </c>
@@ -1783,14 +2176,19 @@
       <c r="D65" s="12">
         <v>437</v>
       </c>
-      <c r="E65" s="35" t="s">
-        <v>24</v>
-      </c>
-      <c r="F65" s="34">
-        <v>539955.80599999998</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E65" s="20"/>
+      <c r="F65" s="20"/>
+      <c r="G65" s="31"/>
+      <c r="H65" s="31"/>
+      <c r="I65" s="31"/>
+      <c r="J65" s="31"/>
+      <c r="K65" s="31"/>
+      <c r="L65" s="31"/>
+      <c r="M65" s="31"/>
+      <c r="N65" s="31"/>
+      <c r="O65" s="31"/>
+    </row>
+    <row r="66" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A66" s="17">
         <v>124</v>
       </c>
@@ -1803,14 +2201,19 @@
       <c r="D66" s="12">
         <v>314</v>
       </c>
-      <c r="E66" s="34">
-        <v>475232.23599999998</v>
-      </c>
-      <c r="F66" s="34">
-        <v>539955.04700000002</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E66" s="20"/>
+      <c r="F66" s="20"/>
+      <c r="G66" s="31"/>
+      <c r="H66" s="31"/>
+      <c r="I66" s="31"/>
+      <c r="J66" s="31"/>
+      <c r="K66" s="31"/>
+      <c r="L66" s="31"/>
+      <c r="M66" s="31"/>
+      <c r="N66" s="31"/>
+      <c r="O66" s="31"/>
+    </row>
+    <row r="67" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A67" s="17">
         <v>81</v>
       </c>
@@ -1823,34 +2226,57 @@
       <c r="D67" s="12">
         <v>342</v>
       </c>
-      <c r="E67" s="34">
-        <v>475233.02799999999</v>
-      </c>
-      <c r="F67" s="34">
-        <v>539954.99300000002</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E67" s="20"/>
+      <c r="F67" s="20"/>
+      <c r="G67" s="31"/>
+      <c r="H67" s="31"/>
+      <c r="I67" s="31"/>
+      <c r="J67" s="31"/>
+      <c r="K67" s="31"/>
+      <c r="L67" s="31"/>
+      <c r="M67" s="31"/>
+      <c r="N67" s="31"/>
+      <c r="O67" s="31"/>
+    </row>
+    <row r="68" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A68" s="17">
         <v>6</v>
       </c>
       <c r="B68" s="12"/>
       <c r="C68" s="12"/>
       <c r="D68" s="12"/>
-      <c r="E68" s="22"/>
-      <c r="F68" s="22"/>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E68" s="20"/>
+      <c r="F68" s="20"/>
+      <c r="G68" s="31"/>
+      <c r="H68" s="31"/>
+      <c r="I68" s="31"/>
+      <c r="J68" s="31"/>
+      <c r="K68" s="31"/>
+      <c r="L68" s="31"/>
+      <c r="M68" s="31"/>
+      <c r="N68" s="31"/>
+      <c r="O68" s="31"/>
+    </row>
+    <row r="69" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A69" s="17">
         <v>11</v>
       </c>
       <c r="B69" s="12"/>
       <c r="C69" s="12"/>
       <c r="D69" s="12"/>
-      <c r="E69" s="22"/>
-      <c r="F69" s="22"/>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E69" s="20"/>
+      <c r="F69" s="20"/>
+      <c r="G69" s="31"/>
+      <c r="H69" s="31"/>
+      <c r="I69" s="31"/>
+      <c r="J69" s="31"/>
+      <c r="K69" s="31"/>
+      <c r="L69" s="31"/>
+      <c r="M69" s="31"/>
+      <c r="N69" s="31"/>
+      <c r="O69" s="31"/>
+    </row>
+    <row r="70" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A70" s="17">
         <v>48</v>
       </c>
@@ -1863,14 +2289,19 @@
       <c r="D70" s="12">
         <v>326</v>
       </c>
-      <c r="E70" s="34">
-        <v>475233.12900000002</v>
-      </c>
-      <c r="F70" s="34">
-        <v>539954.81400000001</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E70" s="20"/>
+      <c r="F70" s="20"/>
+      <c r="G70" s="31"/>
+      <c r="H70" s="31"/>
+      <c r="I70" s="31"/>
+      <c r="J70" s="31"/>
+      <c r="K70" s="31"/>
+      <c r="L70" s="31"/>
+      <c r="M70" s="31"/>
+      <c r="N70" s="31"/>
+      <c r="O70" s="31"/>
+    </row>
+    <row r="71" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A71" s="17">
         <v>62</v>
       </c>
@@ -1883,24 +2314,46 @@
       <c r="D71" s="12">
         <v>276</v>
       </c>
-      <c r="E71" s="34">
-        <v>475232.03700000001</v>
-      </c>
-      <c r="F71" s="34">
-        <v>539954.71600000001</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E71" s="20"/>
+      <c r="F71" s="20"/>
+      <c r="G71" s="31"/>
+      <c r="H71" s="31"/>
+      <c r="I71" s="31"/>
+      <c r="J71" s="31"/>
+      <c r="K71" s="31"/>
+      <c r="L71" s="31"/>
+      <c r="M71" s="31"/>
+      <c r="N71" s="31"/>
+      <c r="O71" s="31"/>
+    </row>
+    <row r="73" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A73" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B73" s="29" t="s">
+      <c r="B73" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="C73" s="29"/>
-      <c r="D73" s="29"/>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C73" s="28"/>
+      <c r="D73" s="28"/>
+      <c r="E73" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="F73" s="29"/>
+      <c r="G73" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="H73" s="29"/>
+      <c r="I73" s="29"/>
+      <c r="J73" s="29"/>
+      <c r="K73" s="29"/>
+      <c r="L73" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="M73" s="29"/>
+      <c r="N73" s="29"/>
+      <c r="O73" s="29"/>
+    </row>
+    <row r="74" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A74" s="10" t="s">
         <v>12</v>
       </c>
@@ -1913,14 +2366,41 @@
       <c r="D74" s="10">
         <v>20</v>
       </c>
-      <c r="E74" s="22" t="s">
+      <c r="E74" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="F74" s="22" t="s">
+      <c r="F74" s="30" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G74" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="H74" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="I74" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="J74" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="K74" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="L74" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="M74" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="N74" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="O74" s="21" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="75" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A75" s="11">
         <v>8</v>
       </c>
@@ -1933,14 +2413,19 @@
       <c r="D75" s="12">
         <v>54</v>
       </c>
-      <c r="E75" s="34">
-        <v>475235.277</v>
-      </c>
-      <c r="F75" s="34">
-        <v>539959.58200000005</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E75" s="20"/>
+      <c r="F75" s="20"/>
+      <c r="G75" s="31"/>
+      <c r="H75" s="31"/>
+      <c r="I75" s="31"/>
+      <c r="J75" s="31"/>
+      <c r="K75" s="31"/>
+      <c r="L75" s="31"/>
+      <c r="M75" s="31"/>
+      <c r="N75" s="31"/>
+      <c r="O75" s="31"/>
+    </row>
+    <row r="76" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A76" s="13">
         <v>2</v>
       </c>
@@ -1953,14 +2438,19 @@
       <c r="D76" s="12">
         <v>100</v>
       </c>
-      <c r="E76" s="34">
-        <v>475235.72399999999</v>
-      </c>
-      <c r="F76" s="34">
-        <v>539959.96900000004</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E76" s="20"/>
+      <c r="F76" s="20"/>
+      <c r="G76" s="31"/>
+      <c r="H76" s="31"/>
+      <c r="I76" s="31"/>
+      <c r="J76" s="31"/>
+      <c r="K76" s="31"/>
+      <c r="L76" s="31"/>
+      <c r="M76" s="31"/>
+      <c r="N76" s="31"/>
+      <c r="O76" s="31"/>
+    </row>
+    <row r="77" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A77" s="13">
         <v>43</v>
       </c>
@@ -1973,14 +2463,19 @@
       <c r="D77" s="12">
         <v>80</v>
       </c>
-      <c r="E77" s="34">
-        <v>475235.35600000003</v>
-      </c>
-      <c r="F77" s="34">
-        <v>539960.272</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E77" s="20"/>
+      <c r="F77" s="20"/>
+      <c r="G77" s="31"/>
+      <c r="H77" s="31"/>
+      <c r="I77" s="31"/>
+      <c r="J77" s="31"/>
+      <c r="K77" s="31"/>
+      <c r="L77" s="31"/>
+      <c r="M77" s="31"/>
+      <c r="N77" s="31"/>
+      <c r="O77" s="31"/>
+    </row>
+    <row r="78" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A78" s="15">
         <v>15</v>
       </c>
@@ -1993,14 +2488,19 @@
       <c r="D78" s="12">
         <v>85</v>
       </c>
-      <c r="E78" s="34">
-        <v>475235.391</v>
-      </c>
-      <c r="F78" s="34">
-        <v>539959.12899999996</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E78" s="20"/>
+      <c r="F78" s="20"/>
+      <c r="G78" s="31"/>
+      <c r="H78" s="31"/>
+      <c r="I78" s="31"/>
+      <c r="J78" s="31"/>
+      <c r="K78" s="31"/>
+      <c r="L78" s="31"/>
+      <c r="M78" s="31"/>
+      <c r="N78" s="31"/>
+      <c r="O78" s="31"/>
+    </row>
+    <row r="79" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A79" s="15">
         <v>94</v>
       </c>
@@ -2013,14 +2513,19 @@
       <c r="D79" s="12">
         <v>73</v>
       </c>
-      <c r="E79" s="34">
-        <v>475235.22399999999</v>
-      </c>
-      <c r="F79" s="34">
-        <v>539959.12699999998</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E79" s="20"/>
+      <c r="F79" s="20"/>
+      <c r="G79" s="31"/>
+      <c r="H79" s="31"/>
+      <c r="I79" s="31"/>
+      <c r="J79" s="31"/>
+      <c r="K79" s="31"/>
+      <c r="L79" s="31"/>
+      <c r="M79" s="31"/>
+      <c r="N79" s="31"/>
+      <c r="O79" s="31"/>
+    </row>
+    <row r="80" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A80" s="15">
         <v>95</v>
       </c>
@@ -2033,14 +2538,19 @@
       <c r="D80" s="12">
         <v>67</v>
       </c>
-      <c r="E80" s="35" t="s">
-        <v>25</v>
-      </c>
-      <c r="F80" s="34">
-        <v>539959.07900000003</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E80" s="20"/>
+      <c r="F80" s="20"/>
+      <c r="G80" s="31"/>
+      <c r="H80" s="31"/>
+      <c r="I80" s="31"/>
+      <c r="J80" s="31"/>
+      <c r="K80" s="31"/>
+      <c r="L80" s="31"/>
+      <c r="M80" s="31"/>
+      <c r="N80" s="31"/>
+      <c r="O80" s="31"/>
+    </row>
+    <row r="81" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A81" s="16">
         <v>109</v>
       </c>
@@ -2053,14 +2563,19 @@
       <c r="D81" s="12">
         <v>75</v>
       </c>
-      <c r="E81" s="34">
-        <v>475235.38799999998</v>
-      </c>
-      <c r="F81" s="34">
-        <v>539960.12800000003</v>
-      </c>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E81" s="20"/>
+      <c r="F81" s="20"/>
+      <c r="G81" s="31"/>
+      <c r="H81" s="31"/>
+      <c r="I81" s="31"/>
+      <c r="J81" s="31"/>
+      <c r="K81" s="31"/>
+      <c r="L81" s="31"/>
+      <c r="M81" s="31"/>
+      <c r="N81" s="31"/>
+      <c r="O81" s="31"/>
+    </row>
+    <row r="82" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A82" s="16">
         <v>66</v>
       </c>
@@ -2073,14 +2588,19 @@
       <c r="D82" s="12">
         <v>148</v>
       </c>
-      <c r="E82" s="34">
-        <v>475234.94300000003</v>
-      </c>
-      <c r="F82" s="34">
-        <v>539958.27099999995</v>
-      </c>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E82" s="20"/>
+      <c r="F82" s="20"/>
+      <c r="G82" s="31"/>
+      <c r="H82" s="31"/>
+      <c r="I82" s="31"/>
+      <c r="J82" s="31"/>
+      <c r="K82" s="31"/>
+      <c r="L82" s="31"/>
+      <c r="M82" s="31"/>
+      <c r="N82" s="31"/>
+      <c r="O82" s="31"/>
+    </row>
+    <row r="83" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A83" s="17">
         <v>73</v>
       </c>
@@ -2088,9 +2608,18 @@
       <c r="C83" s="12"/>
       <c r="D83" s="12"/>
       <c r="E83" s="22"/>
-      <c r="F83" s="22"/>
-    </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F83" s="20"/>
+      <c r="G83" s="31"/>
+      <c r="H83" s="31"/>
+      <c r="I83" s="31"/>
+      <c r="J83" s="31"/>
+      <c r="K83" s="31"/>
+      <c r="L83" s="31"/>
+      <c r="M83" s="31"/>
+      <c r="N83" s="31"/>
+      <c r="O83" s="31"/>
+    </row>
+    <row r="84" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A84" s="17">
         <v>129</v>
       </c>
@@ -2103,14 +2632,19 @@
       <c r="D84" s="12">
         <v>103</v>
       </c>
-      <c r="E84" s="34">
-        <v>475235.22600000002</v>
-      </c>
-      <c r="F84" s="34">
-        <v>539958.80500000005</v>
-      </c>
-    </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E84" s="20"/>
+      <c r="F84" s="20"/>
+      <c r="G84" s="31"/>
+      <c r="H84" s="31"/>
+      <c r="I84" s="31"/>
+      <c r="J84" s="31"/>
+      <c r="K84" s="31"/>
+      <c r="L84" s="31"/>
+      <c r="M84" s="31"/>
+      <c r="N84" s="31"/>
+      <c r="O84" s="31"/>
+    </row>
+    <row r="85" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A85" s="17">
         <v>70</v>
       </c>
@@ -2123,14 +2657,19 @@
       <c r="D85" s="12">
         <v>82</v>
       </c>
-      <c r="E85" s="34">
-        <v>475235.58899999998</v>
-      </c>
-      <c r="F85" s="34">
-        <v>539959.76599999995</v>
-      </c>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E85" s="20"/>
+      <c r="F85" s="20"/>
+      <c r="G85" s="31"/>
+      <c r="H85" s="31"/>
+      <c r="I85" s="31"/>
+      <c r="J85" s="31"/>
+      <c r="K85" s="31"/>
+      <c r="L85" s="31"/>
+      <c r="M85" s="31"/>
+      <c r="N85" s="31"/>
+      <c r="O85" s="31"/>
+    </row>
+    <row r="86" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A86" s="17">
         <v>58</v>
       </c>
@@ -2143,14 +2682,19 @@
       <c r="D86" s="12">
         <v>101</v>
       </c>
-      <c r="E86" s="34">
-        <v>475235.73700000002</v>
-      </c>
-      <c r="F86" s="34">
-        <v>539959.50100000005</v>
-      </c>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E86" s="20"/>
+      <c r="F86" s="20"/>
+      <c r="G86" s="31"/>
+      <c r="H86" s="31"/>
+      <c r="I86" s="31"/>
+      <c r="J86" s="31"/>
+      <c r="K86" s="31"/>
+      <c r="L86" s="31"/>
+      <c r="M86" s="31"/>
+      <c r="N86" s="31"/>
+      <c r="O86" s="31"/>
+    </row>
+    <row r="87" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A87" s="17">
         <v>136</v>
       </c>
@@ -2163,14 +2707,19 @@
       <c r="D87" s="12">
         <v>74</v>
       </c>
-      <c r="E87" s="34">
-        <v>475235.01799999998</v>
-      </c>
-      <c r="F87" s="34">
-        <v>539959.05299999996</v>
-      </c>
-    </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E87" s="20"/>
+      <c r="F87" s="20"/>
+      <c r="G87" s="31"/>
+      <c r="H87" s="31"/>
+      <c r="I87" s="31"/>
+      <c r="J87" s="31"/>
+      <c r="K87" s="31"/>
+      <c r="L87" s="31"/>
+      <c r="M87" s="31"/>
+      <c r="N87" s="31"/>
+      <c r="O87" s="31"/>
+    </row>
+    <row r="88" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A88" s="17">
         <v>39</v>
       </c>
@@ -2183,24 +2732,38 @@
       <c r="D88" s="12">
         <v>110</v>
       </c>
-      <c r="E88" s="34">
-        <v>475235.25300000003</v>
-      </c>
-      <c r="F88" s="34">
-        <v>539958.75899999996</v>
-      </c>
-    </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E88" s="20"/>
+      <c r="F88" s="20"/>
+      <c r="G88" s="31"/>
+      <c r="H88" s="31"/>
+      <c r="I88" s="31"/>
+      <c r="J88" s="31"/>
+      <c r="K88" s="31"/>
+      <c r="L88" s="31"/>
+      <c r="M88" s="31"/>
+      <c r="N88" s="31"/>
+      <c r="O88" s="31"/>
+    </row>
+    <row r="89" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A89" s="17">
         <v>5</v>
       </c>
       <c r="B89" s="12"/>
       <c r="C89" s="12"/>
       <c r="D89" s="12"/>
-      <c r="E89" s="22"/>
-      <c r="F89" s="22"/>
-    </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E89" s="20"/>
+      <c r="F89" s="20"/>
+      <c r="G89" s="31"/>
+      <c r="H89" s="31"/>
+      <c r="I89" s="31"/>
+      <c r="J89" s="31"/>
+      <c r="K89" s="31"/>
+      <c r="L89" s="31"/>
+      <c r="M89" s="31"/>
+      <c r="N89" s="31"/>
+      <c r="O89" s="31"/>
+    </row>
+    <row r="90" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A90" s="17">
         <v>31</v>
       </c>
@@ -2213,34 +2776,65 @@
       <c r="D90" s="12">
         <v>64</v>
       </c>
-      <c r="E90" s="34">
-        <v>475235.40700000001</v>
-      </c>
-      <c r="F90" s="34">
-        <v>539959.59900000005</v>
-      </c>
-    </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E90" s="20"/>
+      <c r="F90" s="20"/>
+      <c r="G90" s="31"/>
+      <c r="H90" s="31"/>
+      <c r="I90" s="31"/>
+      <c r="J90" s="31"/>
+      <c r="K90" s="31"/>
+      <c r="L90" s="31"/>
+      <c r="M90" s="31"/>
+      <c r="N90" s="31"/>
+      <c r="O90" s="31"/>
+    </row>
+    <row r="91" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A91" s="17">
         <v>10</v>
       </c>
       <c r="B91" s="12"/>
       <c r="C91" s="12"/>
       <c r="D91" s="12"/>
-      <c r="E91" s="22"/>
-      <c r="F91" s="22"/>
-    </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E91" s="20"/>
+      <c r="F91" s="20"/>
+      <c r="G91" s="31"/>
+      <c r="H91" s="31"/>
+      <c r="I91" s="31"/>
+      <c r="J91" s="31"/>
+      <c r="K91" s="31"/>
+      <c r="L91" s="31"/>
+      <c r="M91" s="31"/>
+      <c r="N91" s="31"/>
+      <c r="O91" s="31"/>
+    </row>
+    <row r="93" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A93" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B93" s="24" t="s">
+      <c r="B93" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="C93" s="24"/>
-      <c r="D93" s="24"/>
-    </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C93" s="23"/>
+      <c r="D93" s="23"/>
+      <c r="E93" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="F93" s="29"/>
+      <c r="G93" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="H93" s="29"/>
+      <c r="I93" s="29"/>
+      <c r="J93" s="29"/>
+      <c r="K93" s="29"/>
+      <c r="L93" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="M93" s="29"/>
+      <c r="N93" s="29"/>
+      <c r="O93" s="29"/>
+    </row>
+    <row r="94" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A94" s="10" t="s">
         <v>12</v>
       </c>
@@ -2253,14 +2847,41 @@
       <c r="D94" s="10">
         <v>28</v>
       </c>
-      <c r="E94" s="23" t="s">
+      <c r="E94" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="F94" s="23" t="s">
+      <c r="F94" s="30" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G94" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="H94" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="I94" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="J94" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="K94" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="L94" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="M94" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="N94" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="O94" s="21" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="95" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A95" s="11">
         <v>1</v>
       </c>
@@ -2273,14 +2894,19 @@
       <c r="D95" s="12">
         <v>102</v>
       </c>
-      <c r="E95" s="36">
-        <v>475238.82199999999</v>
-      </c>
-      <c r="F95" s="36">
-        <v>539969.28300000005</v>
-      </c>
-    </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E95" s="20"/>
+      <c r="F95" s="20"/>
+      <c r="G95" s="31"/>
+      <c r="H95" s="31"/>
+      <c r="I95" s="31"/>
+      <c r="J95" s="31"/>
+      <c r="K95" s="31"/>
+      <c r="L95" s="31"/>
+      <c r="M95" s="31"/>
+      <c r="N95" s="31"/>
+      <c r="O95" s="31"/>
+    </row>
+    <row r="96" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A96" s="13">
         <v>41</v>
       </c>
@@ -2293,14 +2919,19 @@
       <c r="D96" s="12">
         <v>106</v>
       </c>
-      <c r="E96" s="37" t="s">
-        <v>26</v>
-      </c>
-      <c r="F96" s="36">
-        <v>539968.88100000005</v>
-      </c>
-    </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E96" s="20"/>
+      <c r="F96" s="20"/>
+      <c r="G96" s="31"/>
+      <c r="H96" s="31"/>
+      <c r="I96" s="31"/>
+      <c r="J96" s="31"/>
+      <c r="K96" s="31"/>
+      <c r="L96" s="31"/>
+      <c r="M96" s="31"/>
+      <c r="N96" s="31"/>
+      <c r="O96" s="31"/>
+    </row>
+    <row r="97" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A97" s="15">
         <v>17</v>
       </c>
@@ -2313,14 +2944,19 @@
       <c r="D97" s="12">
         <v>120</v>
       </c>
-      <c r="E97" s="36">
-        <v>475239.03899999999</v>
-      </c>
-      <c r="F97" s="36">
-        <v>539969.26899999997</v>
-      </c>
-    </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E97" s="20"/>
+      <c r="F97" s="20"/>
+      <c r="G97" s="31"/>
+      <c r="H97" s="31"/>
+      <c r="I97" s="31"/>
+      <c r="J97" s="31"/>
+      <c r="K97" s="31"/>
+      <c r="L97" s="31"/>
+      <c r="M97" s="31"/>
+      <c r="N97" s="31"/>
+      <c r="O97" s="31"/>
+    </row>
+    <row r="98" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A98" s="15">
         <v>29</v>
       </c>
@@ -2333,14 +2969,19 @@
       <c r="D98" s="12">
         <v>74</v>
       </c>
-      <c r="E98" s="36">
-        <v>475238.66899999999</v>
-      </c>
-      <c r="F98" s="36">
-        <v>539968.87699999998</v>
-      </c>
-    </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E98" s="20"/>
+      <c r="F98" s="20"/>
+      <c r="G98" s="31"/>
+      <c r="H98" s="31"/>
+      <c r="I98" s="31"/>
+      <c r="J98" s="31"/>
+      <c r="K98" s="31"/>
+      <c r="L98" s="31"/>
+      <c r="M98" s="31"/>
+      <c r="N98" s="31"/>
+      <c r="O98" s="31"/>
+    </row>
+    <row r="99" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A99" s="15">
         <v>14</v>
       </c>
@@ -2353,10 +2994,19 @@
       <c r="D99" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="E99" s="23"/>
-      <c r="F99" s="23"/>
-    </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E99" s="20"/>
+      <c r="F99" s="20"/>
+      <c r="G99" s="31"/>
+      <c r="H99" s="31"/>
+      <c r="I99" s="31"/>
+      <c r="J99" s="31"/>
+      <c r="K99" s="31"/>
+      <c r="L99" s="31"/>
+      <c r="M99" s="31"/>
+      <c r="N99" s="31"/>
+      <c r="O99" s="31"/>
+    </row>
+    <row r="100" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A100" s="16">
         <v>119</v>
       </c>
@@ -2369,14 +3019,19 @@
       <c r="D100" s="12">
         <v>61</v>
       </c>
-      <c r="E100" s="36">
-        <v>475238.56199999998</v>
-      </c>
-      <c r="F100" s="36">
-        <v>539968.78399999999</v>
-      </c>
-    </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E100" s="20"/>
+      <c r="F100" s="20"/>
+      <c r="G100" s="31"/>
+      <c r="H100" s="31"/>
+      <c r="I100" s="31"/>
+      <c r="J100" s="31"/>
+      <c r="K100" s="31"/>
+      <c r="L100" s="31"/>
+      <c r="M100" s="31"/>
+      <c r="N100" s="31"/>
+      <c r="O100" s="31"/>
+    </row>
+    <row r="101" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A101" s="16">
         <v>45</v>
       </c>
@@ -2389,14 +3044,19 @@
       <c r="D101" s="12">
         <v>116</v>
       </c>
-      <c r="E101" s="37" t="s">
-        <v>27</v>
-      </c>
-      <c r="F101" s="36">
-        <v>539968.85600000003</v>
-      </c>
-    </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E101" s="20"/>
+      <c r="F101" s="20"/>
+      <c r="G101" s="31"/>
+      <c r="H101" s="31"/>
+      <c r="I101" s="31"/>
+      <c r="J101" s="31"/>
+      <c r="K101" s="31"/>
+      <c r="L101" s="31"/>
+      <c r="M101" s="31"/>
+      <c r="N101" s="31"/>
+      <c r="O101" s="31"/>
+    </row>
+    <row r="102" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A102" s="16">
         <v>20</v>
       </c>
@@ -2409,14 +3069,19 @@
       <c r="D102" s="12">
         <v>64</v>
       </c>
-      <c r="E102" s="36">
-        <v>475238.59399999998</v>
-      </c>
-      <c r="F102" s="36">
-        <v>539968.68400000001</v>
-      </c>
-    </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E102" s="20"/>
+      <c r="F102" s="20"/>
+      <c r="G102" s="31"/>
+      <c r="H102" s="31"/>
+      <c r="I102" s="31"/>
+      <c r="J102" s="31"/>
+      <c r="K102" s="31"/>
+      <c r="L102" s="31"/>
+      <c r="M102" s="31"/>
+      <c r="N102" s="31"/>
+      <c r="O102" s="31"/>
+    </row>
+    <row r="103" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A103" s="16">
         <v>34</v>
       </c>
@@ -2429,14 +3094,19 @@
       <c r="D103" s="12">
         <v>60</v>
       </c>
-      <c r="E103" s="36">
-        <v>475238.44199999998</v>
-      </c>
-      <c r="F103" s="36">
-        <v>539969.12600000005</v>
-      </c>
-    </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E103" s="22"/>
+      <c r="F103" s="20"/>
+      <c r="G103" s="31"/>
+      <c r="H103" s="31"/>
+      <c r="I103" s="31"/>
+      <c r="J103" s="31"/>
+      <c r="K103" s="31"/>
+      <c r="L103" s="31"/>
+      <c r="M103" s="31"/>
+      <c r="N103" s="31"/>
+      <c r="O103" s="31"/>
+    </row>
+    <row r="104" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A104" s="17">
         <v>64</v>
       </c>
@@ -2449,14 +3119,19 @@
       <c r="D104" s="12">
         <v>65</v>
       </c>
-      <c r="E104" s="36">
-        <v>475238.62900000002</v>
-      </c>
-      <c r="F104" s="36">
-        <v>539968.777</v>
-      </c>
-    </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E104" s="20"/>
+      <c r="F104" s="20"/>
+      <c r="G104" s="31"/>
+      <c r="H104" s="31"/>
+      <c r="I104" s="31"/>
+      <c r="J104" s="31"/>
+      <c r="K104" s="31"/>
+      <c r="L104" s="31"/>
+      <c r="M104" s="31"/>
+      <c r="N104" s="31"/>
+      <c r="O104" s="31"/>
+    </row>
+    <row r="105" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A105" s="17">
         <v>56</v>
       </c>
@@ -2469,54 +3144,95 @@
       <c r="D105" s="12">
         <v>61</v>
       </c>
-      <c r="E105" s="36">
-        <v>475238.45799999998</v>
-      </c>
-      <c r="F105" s="36">
-        <v>539969.09199999995</v>
-      </c>
-    </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E105" s="20"/>
+      <c r="F105" s="20"/>
+      <c r="G105" s="31"/>
+      <c r="H105" s="31"/>
+      <c r="I105" s="31"/>
+      <c r="J105" s="31"/>
+      <c r="K105" s="31"/>
+      <c r="L105" s="31"/>
+      <c r="M105" s="31"/>
+      <c r="N105" s="31"/>
+      <c r="O105" s="31"/>
+    </row>
+    <row r="106" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A106" s="17">
         <v>78</v>
       </c>
       <c r="B106" s="12"/>
       <c r="C106" s="12"/>
       <c r="D106" s="12"/>
-      <c r="E106" s="23"/>
-      <c r="F106" s="23"/>
-    </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E106" s="20"/>
+      <c r="F106" s="20"/>
+      <c r="G106" s="31"/>
+      <c r="H106" s="31"/>
+      <c r="I106" s="31"/>
+      <c r="J106" s="31"/>
+      <c r="K106" s="31"/>
+      <c r="L106" s="31"/>
+      <c r="M106" s="31"/>
+      <c r="N106" s="31"/>
+      <c r="O106" s="31"/>
+    </row>
+    <row r="107" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A107" s="18">
         <v>2</v>
       </c>
       <c r="B107" s="12"/>
       <c r="C107" s="12"/>
       <c r="D107" s="12"/>
-      <c r="E107" s="23"/>
-      <c r="F107" s="23"/>
-    </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E107" s="20"/>
+      <c r="F107" s="20"/>
+      <c r="G107" s="31"/>
+      <c r="H107" s="31"/>
+      <c r="I107" s="31"/>
+      <c r="J107" s="31"/>
+      <c r="K107" s="31"/>
+      <c r="L107" s="31"/>
+      <c r="M107" s="31"/>
+      <c r="N107" s="31"/>
+      <c r="O107" s="31"/>
+    </row>
+    <row r="108" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A108" s="18">
         <v>14</v>
       </c>
       <c r="B108" s="12"/>
       <c r="C108" s="12"/>
       <c r="D108" s="12"/>
-      <c r="E108" s="23"/>
-      <c r="F108" s="23"/>
-    </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E108" s="20"/>
+      <c r="F108" s="20"/>
+      <c r="G108" s="31"/>
+      <c r="H108" s="31"/>
+      <c r="I108" s="31"/>
+      <c r="J108" s="31"/>
+      <c r="K108" s="31"/>
+      <c r="L108" s="31"/>
+      <c r="M108" s="31"/>
+      <c r="N108" s="31"/>
+      <c r="O108" s="31"/>
+    </row>
+    <row r="109" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A109" s="18">
         <v>43</v>
       </c>
       <c r="B109" s="12"/>
       <c r="C109" s="12"/>
       <c r="D109" s="12"/>
-      <c r="E109" s="23"/>
-      <c r="F109" s="23"/>
-    </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E109" s="20"/>
+      <c r="F109" s="20"/>
+      <c r="G109" s="31"/>
+      <c r="H109" s="31"/>
+      <c r="I109" s="31"/>
+      <c r="J109" s="31"/>
+      <c r="K109" s="31"/>
+      <c r="L109" s="31"/>
+      <c r="M109" s="31"/>
+      <c r="N109" s="31"/>
+      <c r="O109" s="31"/>
+    </row>
+    <row r="110" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A110" s="18">
         <v>58</v>
       </c>
@@ -2529,15 +3245,35 @@
       <c r="D110" s="12">
         <v>85</v>
       </c>
-      <c r="E110" s="36">
-        <v>475238.77600000001</v>
-      </c>
-      <c r="F110" s="36">
-        <v>539968.87600000005</v>
-      </c>
+      <c r="E110" s="20"/>
+      <c r="F110" s="20"/>
+      <c r="G110" s="31"/>
+      <c r="H110" s="31"/>
+      <c r="I110" s="31"/>
+      <c r="J110" s="31"/>
+      <c r="K110" s="31"/>
+      <c r="L110" s="31"/>
+      <c r="M110" s="31"/>
+      <c r="N110" s="31"/>
+      <c r="O110" s="31"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="21">
+    <mergeCell ref="E93:F93"/>
+    <mergeCell ref="G93:K93"/>
+    <mergeCell ref="L93:O93"/>
+    <mergeCell ref="L51:O51"/>
+    <mergeCell ref="G51:K51"/>
+    <mergeCell ref="E51:F51"/>
+    <mergeCell ref="E73:F73"/>
+    <mergeCell ref="G73:K73"/>
+    <mergeCell ref="L73:O73"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="G7:K7"/>
+    <mergeCell ref="L7:O7"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="G32:K32"/>
+    <mergeCell ref="L32:O32"/>
     <mergeCell ref="B93:D93"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="B7:D7"/>

</xml_diff>